<commit_message>
JoH paper under correction.
</commit_message>
<xml_diff>
--- a/Optimization case study - JoH/ressources/scores.xlsx
+++ b/Optimization case study - JoH/ressources/scores.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -119,13 +119,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3894,21 +3894,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="I73" sqref="I73"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79:E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="8"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -4251,10 +4251,22 @@
       <c r="E26" s="3"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+      <c r="B27" s="3">
+        <f>AVERAGE(B16:B25)</f>
+        <v>31.12163</v>
+      </c>
+      <c r="C27" s="3">
+        <f t="shared" ref="C27:E27" si="10">AVERAGE(C16:C25)</f>
+        <v>32.273551999999995</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" si="10"/>
+        <v>35.818913999999992</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" si="10"/>
+        <v>35.465513999999992</v>
+      </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="3"/>
@@ -4263,14 +4275,14 @@
       <c r="E28" s="3"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="8" t="s">
+      <c r="C29" s="8"/>
+      <c r="D29" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="8"/>
+      <c r="E29" s="9"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
@@ -4432,189 +4444,207 @@
         <v>40.699999999999996</v>
       </c>
       <c r="C42" s="3">
-        <f t="shared" ref="C42:E42" si="10">C31*100</f>
+        <f t="shared" ref="C42:E42" si="11">C31*100</f>
         <v>39.800000000000004</v>
       </c>
       <c r="D42" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>45.487969999999997</v>
       </c>
       <c r="E42" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>43.766420000000004</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="3">
-        <f t="shared" ref="B43:E43" si="11">B32*100</f>
+        <f t="shared" ref="B43:E43" si="12">B32*100</f>
         <v>38.200000000000003</v>
       </c>
       <c r="C43" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>37.299999999999997</v>
       </c>
       <c r="D43" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>42.447839999999999</v>
       </c>
       <c r="E43" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>40.797750000000001</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="3">
-        <f t="shared" ref="B44:E44" si="12">B33*100</f>
+        <f t="shared" ref="B44:E44" si="13">B33*100</f>
         <v>36.6</v>
       </c>
       <c r="C44" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>34.799999999999997</v>
       </c>
       <c r="D44" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>41.445549999999997</v>
       </c>
       <c r="E44" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>38.964219999999997</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="3">
-        <f t="shared" ref="B45:E45" si="13">B34*100</f>
+        <f t="shared" ref="B45:E45" si="14">B34*100</f>
         <v>32.200000000000003</v>
       </c>
       <c r="C45" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>32.9</v>
       </c>
       <c r="D45" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>36.147939999999998</v>
       </c>
       <c r="E45" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>36.42944</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="3">
-        <f t="shared" ref="B46:E46" si="14">B35*100</f>
+        <f t="shared" ref="B46:E46" si="15">B35*100</f>
         <v>34.300000000000004</v>
       </c>
       <c r="C46" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>38</v>
       </c>
       <c r="D46" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>38.589970000000001</v>
       </c>
       <c r="E46" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>41.411259999999999</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="3">
-        <f t="shared" ref="B47:E47" si="15">B36*100</f>
+        <f t="shared" ref="B47:E47" si="16">B36*100</f>
         <v>36.700000000000003</v>
       </c>
       <c r="C47" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>41.099999999999994</v>
       </c>
       <c r="D47" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>40.95234</v>
       </c>
       <c r="E47" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>44.495939999999997</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="3">
-        <f t="shared" ref="B48:E48" si="16">B37*100</f>
+        <f t="shared" ref="B48:E48" si="17">B37*100</f>
         <v>28.199999999999996</v>
       </c>
       <c r="C48" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>29.9</v>
       </c>
       <c r="D48" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>33.807960000000001</v>
       </c>
       <c r="E48" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>34.573740000000001</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="3">
-        <f t="shared" ref="B49:E49" si="17">B38*100</f>
+        <f t="shared" ref="B49:E49" si="18">B38*100</f>
         <v>34.1</v>
       </c>
       <c r="C49" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>37.9</v>
       </c>
       <c r="D49" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>40.711979999999997</v>
       </c>
       <c r="E49" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>43.081879999999998</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="3">
-        <f t="shared" ref="B50:E50" si="18">B39*100</f>
+        <f t="shared" ref="B50:E50" si="19">B39*100</f>
         <v>33.200000000000003</v>
       </c>
       <c r="C50" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>31.8</v>
       </c>
       <c r="D50" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>38.416869999999996</v>
       </c>
       <c r="E50" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>36.623240000000003</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="3">
-        <f t="shared" ref="B51:E51" si="19">B40*100</f>
+        <f t="shared" ref="B51:E51" si="20">B40*100</f>
         <v>37.799999999999997</v>
       </c>
       <c r="C51" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>38.6</v>
       </c>
       <c r="D51" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>42.632469999999998</v>
       </c>
       <c r="E51" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>42.940190000000001</v>
       </c>
     </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="3">
+        <f>AVERAGE(B42:B51)</f>
+        <v>35.200000000000003</v>
+      </c>
+      <c r="C53" s="3">
+        <f t="shared" ref="C53:E53" si="21">AVERAGE(C42:C51)</f>
+        <v>36.21</v>
+      </c>
+      <c r="D53" s="3">
+        <f t="shared" si="21"/>
+        <v>40.064089000000003</v>
+      </c>
+      <c r="E53" s="3">
+        <f t="shared" si="21"/>
+        <v>40.308408</v>
+      </c>
+    </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" s="7" t="s">
+      <c r="B55" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C55" s="7"/>
-      <c r="D55" s="8" t="s">
+      <c r="C55" s="8"/>
+      <c r="D55" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E55" s="8"/>
+      <c r="E55" s="9"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" s="6" t="s">
@@ -4776,321 +4806,339 @@
         <v>40.699999999999996</v>
       </c>
       <c r="C68" s="3">
-        <f t="shared" ref="C68:E68" si="20">C57*100</f>
+        <f t="shared" ref="C68:E68" si="22">C57*100</f>
         <v>39.800000000000004</v>
       </c>
       <c r="D68" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>45.9</v>
       </c>
       <c r="E68" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>43.6</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="3">
-        <f t="shared" ref="B69:E69" si="21">B58*100</f>
+        <f t="shared" ref="B69:E69" si="23">B58*100</f>
         <v>38.200000000000003</v>
       </c>
       <c r="C69" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>37.299999999999997</v>
       </c>
       <c r="D69" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>42.9</v>
       </c>
       <c r="E69" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>41.3</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="3">
-        <f t="shared" ref="B70:E70" si="22">B59*100</f>
+        <f t="shared" ref="B70:E70" si="24">B59*100</f>
         <v>36.6</v>
       </c>
       <c r="C70" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>34.799999999999997</v>
       </c>
       <c r="D70" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>41.8</v>
       </c>
       <c r="E70" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>39.5</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="3">
-        <f t="shared" ref="B71:E71" si="23">B60*100</f>
+        <f t="shared" ref="B71:E71" si="25">B60*100</f>
         <v>32.200000000000003</v>
       </c>
       <c r="C71" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>32.9</v>
       </c>
       <c r="D71" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>36.799999999999997</v>
       </c>
       <c r="E71" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>37.1</v>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B72" s="3">
-        <f t="shared" ref="B72:E72" si="24">B61*100</f>
+        <f t="shared" ref="B72:E72" si="26">B61*100</f>
         <v>34.300000000000004</v>
       </c>
       <c r="C72" s="3">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>38</v>
       </c>
       <c r="D72" s="3">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>39.200000000000003</v>
       </c>
       <c r="E72" s="3">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>41.8</v>
       </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B73" s="3">
-        <f t="shared" ref="B73:E73" si="25">B62*100</f>
+        <f t="shared" ref="B73:E73" si="27">B62*100</f>
         <v>36.700000000000003</v>
       </c>
       <c r="C73" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>41.099999999999994</v>
       </c>
       <c r="D73" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>41.9</v>
       </c>
       <c r="E73" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>44.6</v>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74" s="3">
-        <f t="shared" ref="B74:E74" si="26">B63*100</f>
+        <f t="shared" ref="B74:E74" si="28">B63*100</f>
         <v>28.199999999999996</v>
       </c>
       <c r="C74" s="3">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>29.9</v>
       </c>
       <c r="D74" s="3">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>34.4</v>
       </c>
       <c r="E74" s="3">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>34.799999999999997</v>
       </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B75" s="3">
-        <f t="shared" ref="B75:E75" si="27">B64*100</f>
+        <f t="shared" ref="B75:E75" si="29">B64*100</f>
         <v>34.1</v>
       </c>
       <c r="C75" s="3">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>37.9</v>
       </c>
       <c r="D75" s="3">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>41.199999999999996</v>
       </c>
       <c r="E75" s="3">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>43.3</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76" s="3">
-        <f t="shared" ref="B76:E76" si="28">B65*100</f>
+        <f t="shared" ref="B76:E76" si="30">B65*100</f>
         <v>33.200000000000003</v>
       </c>
       <c r="C76" s="3">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>31.8</v>
       </c>
       <c r="D76" s="3">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>38.700000000000003</v>
       </c>
       <c r="E76" s="3">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>36.299999999999997</v>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B77" s="3">
-        <f t="shared" ref="B77:E77" si="29">B66*100</f>
+        <f t="shared" ref="B77:E77" si="31">B66*100</f>
         <v>37.799999999999997</v>
       </c>
       <c r="C77" s="3">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>38.6</v>
       </c>
       <c r="D77" s="3">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>43.3</v>
       </c>
       <c r="E77" s="3">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>43.2</v>
       </c>
     </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B79" s="3">
+        <f>AVERAGE(B68:B77)</f>
+        <v>35.200000000000003</v>
+      </c>
+      <c r="C79" s="3">
+        <f t="shared" ref="C79:E79" si="32">AVERAGE(C68:C77)</f>
+        <v>36.21</v>
+      </c>
+      <c r="D79" s="3">
+        <f t="shared" si="32"/>
+        <v>40.61</v>
+      </c>
+      <c r="E79" s="3">
+        <f t="shared" si="32"/>
+        <v>40.549999999999997</v>
+      </c>
+    </row>
     <row r="81" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D81" s="9">
+      <c r="D81" s="7">
         <f>D68-D42</f>
         <v>0.41203000000000145</v>
       </c>
-      <c r="E81" s="9">
+      <c r="E81" s="7">
         <f>E68-E42</f>
         <v>-0.16642000000000223</v>
       </c>
     </row>
     <row r="82" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D82" s="9">
-        <f t="shared" ref="D82:E82" si="30">D69-D43</f>
+      <c r="D82" s="7">
+        <f t="shared" ref="D82:E82" si="33">D69-D43</f>
         <v>0.45215999999999923</v>
       </c>
-      <c r="E82" s="9">
-        <f t="shared" si="30"/>
+      <c r="E82" s="7">
+        <f t="shared" si="33"/>
         <v>0.50224999999999653</v>
       </c>
     </row>
     <row r="83" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D83" s="9">
-        <f t="shared" ref="D83:E83" si="31">D70-D44</f>
+      <c r="D83" s="7">
+        <f t="shared" ref="D83:E83" si="34">D70-D44</f>
         <v>0.35444999999999993</v>
       </c>
-      <c r="E83" s="9">
-        <f t="shared" si="31"/>
+      <c r="E83" s="7">
+        <f t="shared" si="34"/>
         <v>0.53578000000000259</v>
       </c>
     </row>
     <row r="84" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D84" s="9">
-        <f t="shared" ref="D84:E84" si="32">D71-D45</f>
+      <c r="D84" s="7">
+        <f t="shared" ref="D84:E84" si="35">D71-D45</f>
         <v>0.65205999999999875</v>
       </c>
-      <c r="E84" s="9">
-        <f t="shared" si="32"/>
+      <c r="E84" s="7">
+        <f t="shared" si="35"/>
         <v>0.67056000000000182</v>
       </c>
     </row>
     <row r="85" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D85" s="9">
-        <f t="shared" ref="D85:E85" si="33">D72-D46</f>
+      <c r="D85" s="7">
+        <f t="shared" ref="D85:E85" si="36">D72-D46</f>
         <v>0.61003000000000185</v>
       </c>
-      <c r="E85" s="9">
-        <f t="shared" si="33"/>
+      <c r="E85" s="7">
+        <f t="shared" si="36"/>
         <v>0.38873999999999853</v>
       </c>
     </row>
     <row r="86" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D86" s="9">
-        <f t="shared" ref="D86:E86" si="34">D73-D47</f>
+      <c r="D86" s="7">
+        <f t="shared" ref="D86:E86" si="37">D73-D47</f>
         <v>0.94765999999999906</v>
       </c>
-      <c r="E86" s="9">
-        <f t="shared" si="34"/>
+      <c r="E86" s="7">
+        <f t="shared" si="37"/>
         <v>0.10406000000000404</v>
       </c>
     </row>
     <row r="87" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D87" s="9">
-        <f t="shared" ref="D87:E87" si="35">D74-D48</f>
+      <c r="D87" s="7">
+        <f t="shared" ref="D87:E87" si="38">D74-D48</f>
         <v>0.59203999999999724</v>
       </c>
-      <c r="E87" s="9">
-        <f t="shared" si="35"/>
+      <c r="E87" s="7">
+        <f t="shared" si="38"/>
         <v>0.22625999999999635</v>
       </c>
     </row>
     <row r="88" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D88" s="9">
-        <f t="shared" ref="D88:E88" si="36">D75-D49</f>
+      <c r="D88" s="7">
+        <f t="shared" ref="D88:E88" si="39">D75-D49</f>
         <v>0.48801999999999879</v>
       </c>
-      <c r="E88" s="9">
-        <f t="shared" si="36"/>
+      <c r="E88" s="7">
+        <f t="shared" si="39"/>
         <v>0.21811999999999898</v>
       </c>
     </row>
     <row r="89" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D89" s="9">
-        <f t="shared" ref="D89:E89" si="37">D76-D50</f>
+      <c r="D89" s="7">
+        <f t="shared" ref="D89:E89" si="40">D76-D50</f>
         <v>0.28313000000000699</v>
       </c>
-      <c r="E89" s="9">
-        <f t="shared" si="37"/>
+      <c r="E89" s="7">
+        <f t="shared" si="40"/>
         <v>-0.32324000000000552</v>
       </c>
     </row>
     <row r="90" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D90" s="9">
-        <f t="shared" ref="D90:E90" si="38">D77-D51</f>
+      <c r="D90" s="7">
+        <f t="shared" ref="D90:E90" si="41">D77-D51</f>
         <v>0.66752999999999929</v>
       </c>
-      <c r="E90" s="9">
-        <f t="shared" si="38"/>
+      <c r="E90" s="7">
+        <f t="shared" si="41"/>
         <v>0.25981000000000165</v>
       </c>
     </row>
     <row r="91" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D91" s="9"/>
-      <c r="E91" s="9"/>
+      <c r="D91" s="7"/>
+      <c r="E91" s="7"/>
     </row>
     <row r="92" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D92" s="9">
+      <c r="D92" s="7">
         <f>AVERAGE(D81:D90)</f>
         <v>0.54591100000000026</v>
       </c>
-      <c r="E92" s="9">
+      <c r="E92" s="7">
         <f>AVERAGE(E81:E90)</f>
         <v>0.24159199999999928</v>
       </c>
     </row>
     <row r="93" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D93" s="9"/>
-      <c r="E93" s="9"/>
+      <c r="D93" s="7"/>
+      <c r="E93" s="7"/>
     </row>
     <row r="94" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D94" s="9"/>
-      <c r="E94" s="9"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="7"/>
     </row>
     <row r="95" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D95" s="9"/>
-      <c r="E95" s="9"/>
+      <c r="D95" s="7"/>
+      <c r="E95" s="7"/>
     </row>
     <row r="96" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D96" s="9"/>
-      <c r="E96" s="9"/>
+      <c r="D96" s="7"/>
+      <c r="E96" s="7"/>
     </row>
     <row r="97" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D97" s="9"/>
-      <c r="E97" s="9"/>
+      <c r="D97" s="7"/>
+      <c r="E97" s="7"/>
     </row>
     <row r="98" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D98" s="9"/>
-      <c r="E98" s="9"/>
+      <c r="D98" s="7"/>
+      <c r="E98" s="7"/>
     </row>
     <row r="99" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D99" s="9"/>
-      <c r="E99" s="9"/>
+      <c r="D99" s="7"/>
+      <c r="E99" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>